<commit_message>
Maps figures and updates to rosetta
</commit_message>
<xml_diff>
--- a/Planning/Baseline&Timeseries_pops.xlsx
+++ b/Planning/Baseline&Timeseries_pops.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/a_Resurrection/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2E3BF0-137D-BD44-9974-6CB3918F6BCF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379EDA93-4521-354F-8DA3-39BDD5234F8B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{1C7FFBE0-94F5-B840-A910-1A73467688C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="66">
   <si>
-    <t>Site Name</t>
-  </si>
-  <si>
     <t>Lat</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Crane Creek</t>
+  </si>
+  <si>
+    <t>Site_Name</t>
   </si>
 </sst>
 </file>
@@ -230,7 +230,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -295,7 +295,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,21 +636,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>32.899279999999997</v>
@@ -659,12 +659,12 @@
         <v>-116.5849</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>34.28425</v>
@@ -673,12 +673,12 @@
         <v>-117.37539</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>36.690959999999997</v>
@@ -687,12 +687,12 @@
         <v>-118.90961</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>36.200809999999997</v>
@@ -701,12 +701,12 @@
         <v>-118.65092</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>34.07808</v>
@@ -715,12 +715,12 @@
         <v>-116.87558</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>43.37876</v>
@@ -729,12 +729,12 @@
         <v>-122.95207000000001</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>41.80979</v>
@@ -743,12 +743,12 @@
         <v>-123.11887</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>41.665460000000003</v>
@@ -757,12 +757,12 @@
         <v>-123.11341</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>39.742980000000003</v>
@@ -771,12 +771,12 @@
         <v>-120.70401</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>39.394419999999997</v>
@@ -785,12 +785,12 @@
         <v>-121.08302</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>37.539000000000001</v>
@@ -799,12 +799,12 @@
         <v>-119.654</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>42.27411</v>
@@ -813,12 +813,12 @@
         <v>-123.63617000000001</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="10">
         <v>34.065109999999997</v>
@@ -827,12 +827,12 @@
         <v>-118.93279</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>37.157609999999998</v>
@@ -841,12 +841,12 @@
         <v>-118.3334</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1">
         <v>40.43141</v>
@@ -855,12 +855,12 @@
         <v>-123.98378</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>37.776899999999998</v>
@@ -869,12 +869,12 @@
         <v>-120.063</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>38.679879999999997</v>
@@ -883,12 +883,12 @@
         <v>-120.41679000000001</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" ref="B19" si="0">42+(3.23/60)</f>
@@ -899,12 +899,12 @@
         <v>-123.16289999999999</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>37.8100666666667</v>
@@ -913,12 +913,12 @@
         <v>-119.85680000000001</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>33.035960000000003</v>
@@ -927,12 +927,12 @@
         <v>-116.53623</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>39.553840000000001</v>
@@ -941,12 +941,12 @@
         <v>-120.98784999999999</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" ref="B23" si="2">43+(39.6/60)</f>
@@ -957,12 +957,12 @@
         <v>-123.07996666666666</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>32.801220000000001</v>
@@ -971,12 +971,12 @@
         <v>-116.50194</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1">
         <v>42.92653</v>
@@ -985,12 +985,12 @@
         <v>-123.48479</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1">
         <v>38.928809999999999</v>
@@ -999,12 +999,12 @@
         <v>-120.49947</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1">
         <v>41.665460000000003</v>
@@ -1013,12 +1013,12 @@
         <v>-123.11341</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1">
         <v>37.89761</v>
@@ -1027,12 +1027,12 @@
         <v>-121.94553000000001</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1">
         <v>39.122050000000002</v>
@@ -1041,12 +1041,12 @@
         <v>-120.49242</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1">
         <v>39.520400000000002</v>
@@ -1055,12 +1055,12 @@
         <v>-120.99815</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1">
         <v>38.066380000000002</v>
@@ -1069,12 +1069,12 @@
         <v>-120.35368</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1">
         <v>32.65822</v>
@@ -1083,12 +1083,12 @@
         <v>-116.53234999999999</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
         <f>43+(18.349/60)</f>
@@ -1099,12 +1099,12 @@
         <v>-122.95505</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1">
         <v>32.75206</v>
@@ -1113,12 +1113,12 @@
         <v>-116.45220999999999</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
         <v>41.228470000000002</v>
@@ -1127,12 +1127,12 @@
         <v>-123.65159</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1">
         <v>39.712090000000003</v>
@@ -1141,12 +1141,12 @@
         <v>-121.27485</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1">
         <v>34.771709999999999</v>
@@ -1155,12 +1155,12 @@
         <v>-119.94363</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1">
         <v>38.566949999999999</v>
@@ -1169,12 +1169,12 @@
         <v>-120.44067</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="1">
         <v>34.07808</v>
@@ -1183,12 +1183,12 @@
         <v>-116.87558</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="8">
         <f>43+(19.689/60)</f>
@@ -1199,12 +1199,12 @@
         <v>-123.01541666666667</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1">
         <v>38.3872</v>
@@ -1213,12 +1213,12 @@
         <v>-120.21048999999999</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1">
         <v>38.069499999999998</v>
@@ -1227,12 +1227,12 @@
         <v>-122.76317</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1">
         <v>39.99982</v>
@@ -1241,12 +1241,12 @@
         <v>-121.26988</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1">
         <v>36.521050000000002</v>
@@ -1255,12 +1255,12 @@
         <v>-118.89359</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45" s="1">
         <v>36.200809999999997</v>
@@ -1269,12 +1269,12 @@
         <v>-118.65092</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" s="1">
         <v>41.80979</v>
@@ -1283,12 +1283,12 @@
         <v>-123.11887</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="2">
         <v>41.810369999999999</v>
@@ -1297,12 +1297,12 @@
         <v>-123.11668</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>36.517760000000003</v>
@@ -1311,12 +1311,12 @@
         <v>-118.75877</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>37.818800000000003</v>
@@ -1325,12 +1325,12 @@
         <v>-120.007433333333</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1">
         <v>36.690959999999997</v>
@@ -1339,12 +1339,12 @@
         <v>-118.90961</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B51" s="1">
         <v>43.37876</v>
@@ -1353,12 +1353,12 @@
         <v>-122.95207000000001</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1">
         <v>37.203299999999999</v>
@@ -1367,12 +1367,12 @@
         <v>-119.41370000000001</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1">
         <v>41.296900000000001</v>
@@ -1381,12 +1381,12 @@
         <v>-123.36033999999999</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1">
         <v>42.572809999999997</v>
@@ -1395,12 +1395,12 @@
         <v>-124.04742</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1">
         <v>41.250239999999998</v>
@@ -1409,12 +1409,12 @@
         <v>-123.64343</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="1">
         <v>41.87876</v>
@@ -1423,12 +1423,12 @@
         <v>-123.82774000000001</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1">
         <v>39.740009999999998</v>
@@ -1437,12 +1437,12 @@
         <v>-123.63227999999999</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="1">
         <v>43.413699999999999</v>
@@ -1451,12 +1451,12 @@
         <v>-122.78043</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B59" s="1">
         <v>32.89913</v>
@@ -1465,12 +1465,12 @@
         <v>-116.58647000000001</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="1">
         <v>37.743000000000002</v>
@@ -1479,12 +1479,12 @@
         <v>-119.562</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" s="1">
         <v>34.284970000000001</v>
@@ -1493,12 +1493,12 @@
         <v>-117.37862</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" s="1">
         <v>40.658270000000002</v>
@@ -1507,12 +1507,12 @@
         <v>-122.91334000000001</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" s="1">
         <v>37.359200000000001</v>
@@ -1521,12 +1521,12 @@
         <v>-119.34498000000001</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B64" s="1">
         <v>34.28425</v>
@@ -1535,12 +1535,12 @@
         <v>-117.37539</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B65" s="1">
         <v>33.993290000000002</v>
@@ -1549,12 +1549,12 @@
         <v>-116.66267000000001</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B66" s="1">
         <v>38.785400000000003</v>
@@ -1563,12 +1563,12 @@
         <v>-120.21366</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67" s="1">
         <v>46.727339999999998</v>
@@ -1577,12 +1577,12 @@
         <v>-120.82678</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68" s="2">
         <v>42.535290000000003</v>
@@ -1591,12 +1591,12 @@
         <v>-123.73016</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B69" s="2">
         <v>37.703769999999999</v>
@@ -1605,12 +1605,12 @@
         <v>-119.75363</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B70" s="2">
         <v>32.608310000000003</v>
@@ -1619,7 +1619,7 @@
         <v>-116.70098</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>